<commit_message>
Added DrugData table script file
</commit_message>
<xml_diff>
--- a/PMS-Features.xlsx
+++ b/PMS-Features.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GauravO\Documents\Training-Docs\Impact Training\Project\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993D4638-59A8-4E21-8FC5-D9EDF832F479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1534098-02E1-4445-8B74-E066D7FFC504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
-    <sheet name="Common" sheetId="2" r:id="rId2"/>
-    <sheet name="Patient" sheetId="3" r:id="rId3"/>
-    <sheet name="Doctor" sheetId="4" r:id="rId4"/>
-    <sheet name="Nurse" sheetId="5" r:id="rId5"/>
+    <sheet name="Admin" sheetId="6" r:id="rId2"/>
+    <sheet name="Common" sheetId="2" r:id="rId3"/>
+    <sheet name="Patient" sheetId="3" r:id="rId4"/>
+    <sheet name="Doctor" sheetId="4" r:id="rId5"/>
+    <sheet name="Nurse" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>Module</t>
   </si>
@@ -43,9 +44,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>User Login</t>
-  </si>
-  <si>
     <t>Patient</t>
   </si>
   <si>
@@ -64,36 +62,12 @@
     <t>Common</t>
   </si>
   <si>
-    <t>User Authentication</t>
-  </si>
-  <si>
     <t>Story</t>
   </si>
   <si>
-    <t>Create User Login Form and Add Validations</t>
-  </si>
-  <si>
-    <t>Create User Registration Page</t>
-  </si>
-  <si>
-    <t>Create Forgot Password Flow</t>
-  </si>
-  <si>
     <t>Assignee</t>
   </si>
   <si>
-    <t>Patient Profile</t>
-  </si>
-  <si>
-    <t>Create Landing Page for Patient</t>
-  </si>
-  <si>
-    <t>Create Appointment Scheduling tab for patient to schedule an appointment</t>
-  </si>
-  <si>
-    <t>Create Patient inbox tab for patient to view all appointments schedule in calender</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -103,27 +77,9 @@
     <t>Applicable to all(Patient/Doc/Admin)</t>
   </si>
   <si>
-    <t>Create Patient profile tab for Patient to add his demographics and personal details</t>
-  </si>
-  <si>
     <t>Master Data</t>
   </si>
   <si>
-    <t>Design and Create Common Master Tables</t>
-  </si>
-  <si>
-    <t>Create/Design Procedures Table</t>
-  </si>
-  <si>
-    <t>Create/Design Product Table</t>
-  </si>
-  <si>
-    <t>Create/Design Dignosis Table</t>
-  </si>
-  <si>
-    <t>Create/Design Allergies Table</t>
-  </si>
-  <si>
     <t>Common Data ables</t>
   </si>
   <si>
@@ -133,14 +89,119 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Create History Tab about his past appointments</t>
+    <t>Patient Appointments</t>
+  </si>
+  <si>
+    <t>Patient Profile/Patient Details</t>
+  </si>
+  <si>
+    <t>C1 - User Authentication</t>
+  </si>
+  <si>
+    <t>C1.1 - Create User Login Form and Add Validations</t>
+  </si>
+  <si>
+    <t>C1.2 - Create User Registration Page</t>
+  </si>
+  <si>
+    <t>C1.3 - Create Forgot Password Flow</t>
+  </si>
+  <si>
+    <t>C2 - Design and Create Common Master Tables</t>
+  </si>
+  <si>
+    <t>C2.1 - Create/Design Dignosis Table</t>
+  </si>
+  <si>
+    <t>C2.2 - Create/Design Product Table</t>
+  </si>
+  <si>
+    <t>C2.3 - Create/Design Procedures Table</t>
+  </si>
+  <si>
+    <t>C2.4 - Create/Design Allergies Table</t>
+  </si>
+  <si>
+    <t>P1 - Create Landing Page for Patient</t>
+  </si>
+  <si>
+    <t>P2 - Create Patient profile tab for Patient to add his demographics and personal details</t>
+  </si>
+  <si>
+    <t>P3 -Create Appointment Scheduling tab for patient to schedule an appointment</t>
+  </si>
+  <si>
+    <t>P4 - Create Patient inbox tab for patient to view all appointments schedule in calender</t>
+  </si>
+  <si>
+    <t>P5 - Create History Tab about his past appointments</t>
+  </si>
+  <si>
+    <t>P2.1 - Create form for Patient Details to add all demographics &amp; allergies data (refer Use case doc for all form attributes)</t>
+  </si>
+  <si>
+    <t>Patient Details/Visit Details</t>
+  </si>
+  <si>
+    <t>Patient Diagnosis</t>
+  </si>
+  <si>
+    <t>Patient Procedure</t>
+  </si>
+  <si>
+    <t>Patient Medication</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>D1 - Create Landing Page for Doctor</t>
+  </si>
+  <si>
+    <t>N1 - Create Landing Page for Nurse</t>
+  </si>
+  <si>
+    <t>A1 - Create Landing Page For Admin</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Page </t>
+  </si>
+  <si>
+    <t>C3 - Design and create Home Page for Application</t>
+  </si>
+  <si>
+    <t>Charu</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Anmol</t>
+  </si>
+  <si>
+    <t>Sonal</t>
+  </si>
+  <si>
+    <t>User Login/Registration</t>
+  </si>
+  <si>
+    <t>C3.2 - Create Navigation Bar on Home Page with Fields Login/Register/About Us etc</t>
+  </si>
+  <si>
+    <t>C3.1 - Design Home Page and design components hierarchy &amp; Collect/finalize static data like Images/Icons/Typography</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,8 +209,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +232,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,17 +253,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,23 +573,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.81640625" customWidth="1"/>
     <col min="3" max="3" width="52.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="31.90625" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="31.90625" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -492,191 +604,351 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="7"/>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="7"/>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="7"/>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="7"/>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="7"/>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="7"/>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="7"/>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="7"/>
+      <c r="C13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="7"/>
+      <c r="C14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" s="7"/>
+      <c r="C16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="7"/>
+      <c r="C17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="7"/>
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="G19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="E20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>8</v>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -685,6 +957,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC546A6-5D4E-47C4-9A0A-8D9E4ABB3D9C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2ABDDC9-B11B-4EF1-9DC5-3653FA9E4899}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -698,7 +984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB87052B-75BD-4572-939B-1903B559ECB6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -712,7 +998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DC9966-B6D7-48AA-B222-6B508F6FA714}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -726,7 +1012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CAB61C-E013-4550-A7C7-9AC16C08A7F2}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>